<commit_message>
que os mestres do git me perdoem
</commit_message>
<xml_diff>
--- a/modelo.xlsx
+++ b/modelo.xlsx
@@ -400,10 +400,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="167" zoomScaleNormal="167" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -416,8 +416,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="9.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16383" min="16382" style="3" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="3" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -708,22 +707,83 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="1"/>
-      <c r="D17" s="2"/>
-    </row>
+    <row r="1048500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <autoFilter ref="A1:C9"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>